<commit_message>
change to while loop
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80B8DF8-9C5B-C945-8333-FF970674459A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41566117-352A-9F4A-82FD-F5536AD39B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>H-Index</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Hashmap with array methods such as array_rand(), isset(), unset()</t>
+  </si>
+  <si>
+    <t>Product of Array Except Self O(n)</t>
+  </si>
+  <si>
+    <t>Postfix and prefix</t>
   </si>
 </sst>
 </file>
@@ -438,13 +444,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1297833B-B28F-3140-BD70-E3D664D3F8B2}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,6 +510,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>238</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
that wasn't much hard
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37AA519-1100-4C4A-BFB1-2F06D4EF6476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFF0DD2-0B93-284A-A1CB-BEF9751D00D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>H-Index</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Summary Ranges</t>
+  </si>
+  <si>
+    <t>Merge Intetvals</t>
   </si>
 </sst>
 </file>
@@ -781,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -995,6 +998,20 @@
       </c>
       <c r="C20" t="s">
         <v>44</v>
+      </c>
+      <c r="E20" s="5">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
linked list as hash
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9D603C-121B-4048-93CA-2E364B11FF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897E21BD-54C4-2242-B629-F5D82D79143A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>H-Index</t>
   </si>
@@ -236,6 +236,15 @@
   </si>
   <si>
     <t>Linked List Cycle</t>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
+  </si>
+  <si>
+    <t>Include carry</t>
+  </si>
+  <si>
+    <t>Copy List with Random Pointer</t>
   </si>
 </sst>
 </file>
@@ -315,7 +324,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -453,36 +462,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -796,20 +775,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.83203125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="7"/>
+    <col min="5" max="5" width="64.5" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>47</v>
@@ -818,17 +798,20 @@
       <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>2</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>88</v>
       </c>
@@ -838,11 +821,11 @@
       <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="5">
         <v>44256</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>80</v>
       </c>
@@ -852,22 +835,23 @@
       <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F3" s="5">
         <v>44256</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>125</v>
       </c>
@@ -880,11 +864,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <v>44256</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>167</v>
       </c>
@@ -897,22 +881,23 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>44256</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>209</v>
       </c>
@@ -922,22 +907,23 @@
       <c r="C10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="5">
         <v>44256</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>36</v>
       </c>
@@ -947,22 +933,23 @@
       <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="5">
+      <c r="F13" s="5">
         <v>44256</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>383</v>
       </c>
@@ -972,11 +959,11 @@
       <c r="C16" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="5">
+      <c r="F16" s="5">
         <v>44256</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>49</v>
       </c>
@@ -986,22 +973,23 @@
       <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="5">
+      <c r="F17" s="5">
         <v>44621</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>228</v>
       </c>
@@ -1011,11 +999,11 @@
       <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="5">
+      <c r="F20" s="5">
         <v>44621</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>56</v>
       </c>
@@ -1025,22 +1013,23 @@
       <c r="C21" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="5">
+      <c r="F21" s="5">
         <v>44621</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1050,11 +1039,11 @@
       <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="5">
+      <c r="F24" s="5">
         <v>44621</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>71</v>
       </c>
@@ -1064,22 +1053,23 @@
       <c r="C25" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="5">
+      <c r="F25" s="5">
         <v>44621</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="6"/>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>141</v>
       </c>
@@ -1089,12 +1079,49 @@
       <c r="C28" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="5">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="5">
         <v>44986</v>
       </c>
     </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="5">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>138</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E1048576">
+  <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -1110,7 +1137,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
knocking out easy ones
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA5E018-3B91-F042-BFA4-0A032026F99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FA3F2E-1BDC-A444-BF67-E73DD5CCF47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
   <si>
     <t>H-Index</t>
   </si>
@@ -175,6 +175,9 @@
     <t>Easy</t>
   </si>
   <si>
+    <t>Remove Element</t>
+  </si>
+  <si>
     <t>Remove Duplicates from Sorted Array II</t>
   </si>
   <si>
@@ -296,6 +299,15 @@
   </si>
   <si>
     <t>Understand the question better.</t>
+  </si>
+  <si>
+    <t>Clone Graph</t>
+  </si>
+  <si>
+    <t>Hashmap and search.</t>
+  </si>
+  <si>
+    <t>Two pointer</t>
   </si>
 </sst>
 </file>
@@ -739,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,17 +768,17 @@
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1">
         <v>2</v>
@@ -794,53 +806,53 @@
         <v>80</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F3" s="5">
         <v>44256</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>125</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="5">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5">
-        <v>44256</v>
-      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>167</v>
-      </c>
-      <c r="B7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -849,225 +861,222 @@
         <v>44256</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>167</v>
+      </c>
+      <c r="B8" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>44256</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>209</v>
       </c>
-      <c r="B10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="5">
         <v>44256</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="5">
         <v>44256</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>383</v>
-      </c>
-      <c r="B16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="5">
-        <v>44256</v>
-      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>49</v>
+        <v>383</v>
       </c>
       <c r="B17" t="s">
         <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F17" s="5">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="5">
         <v>44621</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>228</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="5">
-        <v>44621</v>
-      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>56</v>
+        <v>228</v>
       </c>
       <c r="B21" t="s">
         <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F21" s="5">
         <v>44621</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="5">
+        <v>44621</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="5">
-        <v>44621</v>
-      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F25" s="5">
         <v>44621</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="5">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>141</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="5">
-        <v>44986</v>
-      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="B29" t="s">
         <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="F29" s="5">
         <v>44986</v>
@@ -1075,73 +1084,79 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>138</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
         <v>68</v>
-      </c>
-      <c r="C30" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" t="s">
-        <v>69</v>
       </c>
       <c r="F30" s="5">
         <v>44986</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>138</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="F31" s="5">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>104</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="B34" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F33" s="5">
-        <v>44986</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>100</v>
-      </c>
-      <c r="B34" t="s">
-        <v>73</v>
       </c>
       <c r="C34" t="s">
         <v>44</v>
       </c>
+      <c r="E34" t="s">
+        <v>73</v>
+      </c>
       <c r="F34" s="5">
         <v>44986</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
         <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F35" s="5">
         <v>44986</v>
@@ -1149,107 +1164,138 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
         <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F36" s="5">
         <v>44986</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>106</v>
+      </c>
+      <c r="B37" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="5">
+        <v>44986</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>530</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C39" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" t="s">
-        <v>78</v>
-      </c>
-      <c r="F39" s="5">
-        <v>44986</v>
-      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>230</v>
+        <v>530</v>
       </c>
       <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" t="s">
         <v>79</v>
-      </c>
-      <c r="C40" t="s">
-        <v>46</v>
-      </c>
-      <c r="E40" t="s">
-        <v>80</v>
       </c>
       <c r="F40" s="5">
         <v>44986</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>230</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="F41" s="5">
+        <v>44986</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>200</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C43" t="s">
-        <v>46</v>
-      </c>
-      <c r="E43" t="s">
-        <v>83</v>
-      </c>
-      <c r="F43" s="5">
-        <v>45352</v>
-      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
+        <v>200</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" t="s">
+        <v>84</v>
+      </c>
+      <c r="F44" s="5">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45">
         <v>130</v>
       </c>
-      <c r="B44" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" t="s">
-        <v>46</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="B45" t="s">
         <v>85</v>
       </c>
-      <c r="F44" s="5">
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" t="s">
+        <v>86</v>
+      </c>
+      <c r="F45" s="5">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46" s="5">
         <v>45717</v>
       </c>
     </row>
@@ -1278,7 +1324,8 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{45809EEC-81DF-6A4E-91D1-93A7E83EA600}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{E8209BAF-E983-F84D-85E9-51122788BE77}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{9D51CCC3-C920-5246-9214-4E41C6EAE383}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{9D51CCC3-C920-5246-9214-4E41C6EAE383}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{123BEFC6-385A-644B-AEEF-1E4E98150A90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
i need some break
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D979F919-48A4-1C4C-9F83-EA81E0FB7FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F09081-E206-EB48-B3AD-4A08A4D3C489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="136">
   <si>
     <t>H-Index</t>
   </si>
@@ -432,6 +432,21 @@
   </si>
   <si>
     <t>Permutations</t>
+  </si>
+  <si>
+    <t>Combination Sum</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>DFS, work on the decision tree</t>
+  </si>
+  <si>
+    <t>Divide and Conquer</t>
+  </si>
+  <si>
+    <t>Convert Sorted Array to BST</t>
   </si>
 </sst>
 </file>
@@ -873,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1809,7 +1824,60 @@
       <c r="C69" t="s">
         <v>48</v>
       </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
       <c r="G69" s="5">
+        <v>46813</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>39</v>
+      </c>
+      <c r="B70" t="s">
+        <v>131</v>
+      </c>
+      <c r="C70" t="s">
+        <v>48</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>133</v>
+      </c>
+      <c r="G70" s="5">
+        <v>46813</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>108</v>
+      </c>
+      <c r="B73" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" t="s">
+        <v>44</v>
+      </c>
+      <c r="F73" t="s">
+        <v>132</v>
+      </c>
+      <c r="G73" s="5">
         <v>46813</v>
       </c>
     </row>

</xml_diff>

<commit_message>
i can do this
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F09081-E206-EB48-B3AD-4A08A4D3C489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3579788-C180-3049-9997-38920FC69AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="139">
   <si>
     <t>H-Index</t>
   </si>
@@ -447,6 +447,15 @@
   </si>
   <si>
     <t>Convert Sorted Array to BST</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Search Insert Position</t>
+  </si>
+  <si>
+    <t>Think about what to return when there is no found</t>
   </si>
 </sst>
 </file>
@@ -888,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1878,6 +1887,33 @@
         <v>132</v>
       </c>
       <c r="G73" s="5">
+        <v>46813</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>137</v>
+      </c>
+      <c r="C76" t="s">
+        <v>44</v>
+      </c>
+      <c r="F76" t="s">
+        <v>138</v>
+      </c>
+      <c r="G76" s="5">
         <v>46813</v>
       </c>
     </row>

</xml_diff>

<commit_message>
getting good at dfs as well
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E944AE2-759D-FB45-B0F1-48EE7F287F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EDDB00-B2E7-5140-A7AD-03AA6CE54312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="34560" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="171">
   <si>
     <t>H-Index</t>
   </si>
@@ -546,6 +546,12 @@
   </si>
   <si>
     <t>Reverse pyramid</t>
+  </si>
+  <si>
+    <t>Unique Path II</t>
+  </si>
+  <si>
+    <t>Out of range grid technique</t>
   </si>
 </sst>
 </file>
@@ -991,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2305,6 +2311,23 @@
         <v>168</v>
       </c>
       <c r="G97" s="7">
+        <v>37712</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>63</v>
+      </c>
+      <c r="B98" t="s">
+        <v>169</v>
+      </c>
+      <c r="C98" t="s">
+        <v>48</v>
+      </c>
+      <c r="F98" t="s">
+        <v>170</v>
+      </c>
+      <c r="G98" s="7">
         <v>37712</v>
       </c>
     </row>

</xml_diff>

<commit_message>
i need some candy
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A4206E-1984-E240-B016-73AF670A46C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8399C8A3-FE58-1E4D-8F19-71D3AB492147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I97" sqref="I97"/>
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
recursion is hard af
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECF1446-D466-814B-93AD-030A6A14D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF3F863-851B-3244-B997-528B8FB8FA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10600" yWindow="760" windowWidth="23960" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="189">
   <si>
     <t>H-Index</t>
   </si>
@@ -600,6 +600,12 @@
   </si>
   <si>
     <t xml:space="preserve">Remove Duplicate from Sorted List </t>
+  </si>
+  <si>
+    <t>Hashmap and Two iterations</t>
+  </si>
+  <si>
+    <t>Flatten Binary Tree to Linked List</t>
   </si>
 </sst>
 </file>
@@ -691,7 +697,17 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1122,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1851,6 +1867,12 @@
       <c r="C52" t="s">
         <v>48</v>
       </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>187</v>
+      </c>
       <c r="G52" s="7">
         <v>38443</v>
       </c>
@@ -1937,11 +1959,17 @@
       <c r="C59" t="s">
         <v>44</v>
       </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
       <c r="F59" t="s">
         <v>106</v>
       </c>
       <c r="G59" s="7">
         <v>46082</v>
+      </c>
+      <c r="H59" s="7">
+        <v>38443</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -2004,48 +2032,39 @@
         <v>46447</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>114</v>
+      </c>
+      <c r="B63" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>530</v>
-      </c>
-      <c r="B65" t="s">
-        <v>78</v>
-      </c>
-      <c r="C65" t="s">
-        <v>44</v>
-      </c>
-      <c r="F65" t="s">
-        <v>79</v>
-      </c>
-      <c r="G65" s="7">
-        <v>44986</v>
-      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>230</v>
+        <v>530</v>
       </c>
       <c r="B66" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C66" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F66" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G66" s="7">
         <v>44986</v>
@@ -2053,80 +2072,80 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
+        <v>230</v>
+      </c>
+      <c r="B67" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" t="s">
+        <v>48</v>
+      </c>
+      <c r="F67" t="s">
+        <v>81</v>
+      </c>
+      <c r="G67" s="7">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68">
         <v>98</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>117</v>
       </c>
-      <c r="C67" t="s">
-        <v>48</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="C68" t="s">
+        <v>48</v>
+      </c>
+      <c r="F68" t="s">
         <v>121</v>
       </c>
-      <c r="G67" s="7">
+      <c r="G68" s="7">
         <v>46447</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1" t="s">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>200</v>
-      </c>
-      <c r="B70" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" t="s">
-        <v>48</v>
-      </c>
-      <c r="F70" t="s">
-        <v>84</v>
-      </c>
-      <c r="G70" s="7">
-        <v>45352</v>
-      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="B71" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
         <v>48</v>
       </c>
       <c r="F71" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G71" s="7">
-        <v>45717</v>
+        <v>45352</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B72" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C72" t="s">
         <v>48</v>
       </c>
       <c r="F72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G72" s="7">
         <v>45717</v>
@@ -2134,36 +2153,33 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>909</v>
+        <v>133</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="C73" t="s">
         <v>48</v>
       </c>
       <c r="F73" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="G73" s="7">
-        <v>46447</v>
+        <v>45717</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>399</v>
+        <v>909</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C74" t="s">
         <v>48</v>
       </c>
-      <c r="E74">
-        <v>1</v>
-      </c>
       <c r="F74" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G74" s="7">
         <v>46447</v>
@@ -2171,10 +2187,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>207</v>
+        <v>399</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C75" t="s">
         <v>48</v>
@@ -2182,46 +2198,49 @@
       <c r="E75">
         <v>1</v>
       </c>
+      <c r="F75" t="s">
+        <v>110</v>
+      </c>
       <c r="G75" s="7">
         <v>46447</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1" t="s">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>207</v>
+      </c>
+      <c r="B76" t="s">
+        <v>116</v>
+      </c>
+      <c r="C76" t="s">
+        <v>48</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="G76" s="7">
+        <v>46447</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="6"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>17</v>
-      </c>
-      <c r="B78" t="s">
-        <v>125</v>
-      </c>
-      <c r="C78" t="s">
-        <v>48</v>
-      </c>
-      <c r="F78" t="s">
-        <v>126</v>
-      </c>
-      <c r="G78" s="7">
-        <v>46447</v>
-      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C79" t="s">
         <v>48</v>
@@ -2235,27 +2254,27 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="B80" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C80" t="s">
         <v>48</v>
       </c>
-      <c r="E80">
-        <v>1</v>
+      <c r="F80" t="s">
+        <v>126</v>
       </c>
       <c r="G80" s="7">
-        <v>46813</v>
+        <v>46447</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B81" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C81" t="s">
         <v>48</v>
@@ -2263,85 +2282,85 @@
       <c r="E81">
         <v>1</v>
       </c>
-      <c r="F81" t="s">
-        <v>131</v>
-      </c>
       <c r="G81" s="7">
         <v>46813</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1" t="s">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>39</v>
+      </c>
+      <c r="B82" t="s">
+        <v>129</v>
+      </c>
+      <c r="C82" t="s">
+        <v>48</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82" t="s">
+        <v>131</v>
+      </c>
+      <c r="G82" s="7">
+        <v>46813</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="6"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84">
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85">
         <v>108</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>133</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>44</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F85" t="s">
         <v>130</v>
       </c>
-      <c r="G84" s="7">
+      <c r="G85" s="7">
         <v>46813</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="6"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>35</v>
-      </c>
-      <c r="B87" t="s">
-        <v>135</v>
-      </c>
-      <c r="C87" t="s">
-        <v>44</v>
-      </c>
-      <c r="F87" t="s">
-        <v>136</v>
-      </c>
-      <c r="G87" s="7">
-        <v>46813</v>
-      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="B88" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C88" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F88" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G88" s="7">
         <v>46813</v>
@@ -2349,16 +2368,16 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="B89" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C89" t="s">
         <v>48</v>
       </c>
       <c r="F89" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G89" s="7">
         <v>46813</v>
@@ -2366,16 +2385,16 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="B90" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C90" t="s">
         <v>48</v>
       </c>
       <c r="F90" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G90" s="7">
         <v>46813</v>
@@ -2383,171 +2402,171 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91">
+        <v>33</v>
+      </c>
+      <c r="B91" t="s">
+        <v>141</v>
+      </c>
+      <c r="C91" t="s">
+        <v>48</v>
+      </c>
+      <c r="F91" t="s">
+        <v>142</v>
+      </c>
+      <c r="G91" s="7">
+        <v>46813</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92">
         <v>34</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>143</v>
       </c>
-      <c r="C91" t="s">
-        <v>48</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="C92" t="s">
+        <v>48</v>
+      </c>
+      <c r="F92" t="s">
         <v>144</v>
       </c>
-      <c r="G91" s="7">
+      <c r="G92" s="7">
         <v>47178</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="6"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>215</v>
-      </c>
-      <c r="B94" t="s">
-        <v>146</v>
-      </c>
-      <c r="C94" t="s">
-        <v>48</v>
-      </c>
-      <c r="F94" t="s">
-        <v>147</v>
-      </c>
-      <c r="G94" s="7">
-        <v>47178</v>
-      </c>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>373</v>
+        <v>215</v>
       </c>
       <c r="B95" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C95" t="s">
         <v>48</v>
       </c>
-      <c r="E95">
-        <v>1</v>
+      <c r="F95" t="s">
+        <v>147</v>
       </c>
       <c r="G95" s="7">
         <v>47178</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1" t="s">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>373</v>
+      </c>
+      <c r="B96" t="s">
+        <v>148</v>
+      </c>
+      <c r="C96" t="s">
+        <v>48</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="G96" s="7">
+        <v>47178</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
-      <c r="G97" s="6"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>67</v>
-      </c>
-      <c r="B98" t="s">
-        <v>150</v>
-      </c>
-      <c r="C98" t="s">
-        <v>44</v>
-      </c>
-      <c r="F98" t="s">
-        <v>151</v>
-      </c>
-      <c r="G98" s="7">
-        <v>47178</v>
-      </c>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>190</v>
+        <v>67</v>
       </c>
       <c r="B99" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C99" t="s">
         <v>44</v>
       </c>
       <c r="F99" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G99" s="7">
-        <v>11018</v>
+        <v>47178</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>136</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C100" t="s">
         <v>44</v>
       </c>
       <c r="F100" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G100" s="7">
         <v>11018</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1" t="s">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>136</v>
+      </c>
+      <c r="B101" t="s">
+        <v>154</v>
+      </c>
+      <c r="C101" t="s">
+        <v>44</v>
+      </c>
+      <c r="F101" t="s">
+        <v>155</v>
+      </c>
+      <c r="G101" s="7">
+        <v>11018</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="6"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <v>70</v>
-      </c>
-      <c r="B103" t="s">
-        <v>157</v>
-      </c>
-      <c r="C103" t="s">
-        <v>44</v>
-      </c>
-      <c r="G103" s="7">
-        <v>11018</v>
-      </c>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>198</v>
+        <v>70</v>
       </c>
       <c r="B104" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C104" t="s">
-        <v>48</v>
-      </c>
-      <c r="F104" t="s">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="G104" s="7">
         <v>11018</v>
@@ -2555,50 +2574,53 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>139</v>
+        <v>198</v>
       </c>
       <c r="B105" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C105" t="s">
         <v>48</v>
       </c>
-      <c r="E105">
-        <v>1</v>
-      </c>
       <c r="F105" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G105" s="7">
-        <v>11383</v>
+        <v>11018</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>322</v>
+        <v>139</v>
       </c>
       <c r="B106" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C106" t="s">
         <v>48</v>
       </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
       <c r="F106" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G106" s="7">
-        <v>37347</v>
+        <v>11383</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>300</v>
+        <v>322</v>
       </c>
       <c r="B107" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C107" t="s">
         <v>48</v>
+      </c>
+      <c r="F107" t="s">
+        <v>163</v>
       </c>
       <c r="G107" s="7">
         <v>37347</v>
@@ -2606,39 +2628,33 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="B108" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C108" t="s">
         <v>48</v>
       </c>
-      <c r="E108">
-        <v>1</v>
-      </c>
-      <c r="F108" t="s">
-        <v>166</v>
-      </c>
       <c r="G108" s="7">
-        <v>37712</v>
-      </c>
-      <c r="H108" s="7">
-        <v>38078</v>
+        <v>37347</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="B109" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C109" t="s">
         <v>48</v>
       </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
       <c r="F109" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G109" s="7">
         <v>37712</v>
@@ -2649,74 +2665,99 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110">
+        <v>63</v>
+      </c>
+      <c r="B110" t="s">
+        <v>167</v>
+      </c>
+      <c r="C110" t="s">
+        <v>48</v>
+      </c>
+      <c r="F110" t="s">
+        <v>168</v>
+      </c>
+      <c r="G110" s="7">
+        <v>37712</v>
+      </c>
+      <c r="H110" s="7">
+        <v>38078</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111">
         <v>97</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>169</v>
       </c>
-      <c r="C110" t="s">
-        <v>48</v>
-      </c>
-      <c r="F110" t="s">
+      <c r="C111" t="s">
+        <v>48</v>
+      </c>
+      <c r="F111" t="s">
         <v>170</v>
       </c>
-      <c r="G110" s="7">
+      <c r="G111" s="7">
         <v>38078</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F43:F76 F1:F39 D1:E76 D77:F1048576">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+  <conditionalFormatting sqref="F43:F77 F1:F39 D1:E77 D78:F1048576">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G42 G44:G49 G53:G1048576">
-    <cfRule type="cellIs" dxfId="7" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="13" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H109">
     <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H108">
+  <conditionalFormatting sqref="H110">
     <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H109">
+  <conditionalFormatting sqref="H39">
     <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
+  <conditionalFormatting sqref="H45">
     <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H45">
+  <conditionalFormatting sqref="H47:H48">
     <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47:H48">
+  <conditionalFormatting sqref="G50:G52">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G50:G52">
+  <conditionalFormatting sqref="H59">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
getting good with tree
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DAD08E-C32A-9540-93FC-72C948CA4FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7864F936-9D3C-6C41-9135-46918B835345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10600" yWindow="760" windowWidth="23960" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -709,7 +709,27 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1152,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2124,6 +2144,9 @@
       <c r="G68" s="7">
         <v>44986</v>
       </c>
+      <c r="H68" s="7">
+        <v>38808</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
@@ -2135,11 +2158,17 @@
       <c r="C69" t="s">
         <v>48</v>
       </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
       <c r="F69" t="s">
         <v>81</v>
       </c>
       <c r="G69" s="7">
         <v>44986</v>
+      </c>
+      <c r="H69" s="7">
+        <v>38808</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -2757,62 +2786,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F39 F43:F65 D1:E65 D64:F1048576">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G42 G44:G49 G53:G1048576">
-    <cfRule type="cellIs" dxfId="8" priority="13" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="15" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H111">
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H112">
     <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H111">
+  <conditionalFormatting sqref="H39">
     <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H112">
+  <conditionalFormatting sqref="H45">
     <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
+  <conditionalFormatting sqref="H47:H48">
     <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H45">
+  <conditionalFormatting sqref="G50:G52">
     <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47:H48">
+  <conditionalFormatting sqref="H59">
     <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G50:G52">
+  <conditionalFormatting sqref="H68">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H59">
+  <conditionalFormatting sqref="H69">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
getting good at dfs
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E5EEA2-52A8-D04B-BEC8-56CF6640086F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5694E354-73FC-C041-BB27-945D9FECF0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12120" yWindow="760" windowWidth="22440" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -399,9 +399,6 @@
     <t>Word Break</t>
   </si>
   <si>
-    <t>What da..</t>
-  </si>
-  <si>
     <t>Coin Change</t>
   </si>
   <si>
@@ -562,6 +559,9 @@
   </si>
   <si>
     <t>What da fuck…?</t>
+  </si>
+  <si>
+    <t>Bottom up, find the base case and work from there on dp table</t>
   </si>
 </sst>
 </file>
@@ -1279,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="G1" s="8">
         <f>COUNTA(G2:I176)</f>
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1393,7 +1393,7 @@
         <v>121</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1410,13 +1410,13 @@
         <v>122</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
         <v>131</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>132</v>
       </c>
       <c r="G8" s="6">
         <v>38078</v>
@@ -1497,7 +1497,7 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G14" s="6">
         <v>38078</v>
@@ -1588,7 +1588,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G23" s="6">
         <v>46082</v>
@@ -1602,13 +1602,13 @@
         <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G24" s="6">
         <v>38078</v>
@@ -1666,7 +1666,7 @@
         <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G29" s="6">
         <v>38078</v>
@@ -1699,7 +1699,7 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G32" s="6">
         <v>44621</v>
@@ -1744,7 +1744,7 @@
         <v>452</v>
       </c>
       <c r="B35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -1753,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G35" s="6">
         <v>38443</v>
@@ -1907,7 +1907,7 @@
         <v>11</v>
       </c>
       <c r="F47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G47" s="6">
         <v>44986</v>
@@ -1961,13 +1961,13 @@
         <v>206</v>
       </c>
       <c r="B50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
       </c>
       <c r="F50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G50" s="6">
         <v>38443</v>
@@ -1978,7 +1978,7 @@
         <v>83</v>
       </c>
       <c r="B51" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -1998,7 +1998,7 @@
         <v>82</v>
       </c>
       <c r="B52" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
         <v>11</v>
@@ -2007,7 +2007,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G52" s="6">
         <v>38443</v>
@@ -2173,13 +2173,13 @@
         <v>114</v>
       </c>
       <c r="B63" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" t="s">
         <v>147</v>
-      </c>
-      <c r="C63" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" t="s">
-        <v>148</v>
       </c>
       <c r="G63" s="6">
         <v>38808</v>
@@ -2190,13 +2190,13 @@
         <v>199</v>
       </c>
       <c r="B64" t="s">
+        <v>148</v>
+      </c>
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" t="s">
         <v>149</v>
-      </c>
-      <c r="C64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" t="s">
-        <v>150</v>
       </c>
       <c r="G64" s="6">
         <v>38808</v>
@@ -2207,7 +2207,7 @@
         <v>637</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C65" t="s">
         <v>7</v>
@@ -2376,7 +2376,7 @@
         <v>11</v>
       </c>
       <c r="F76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G76" s="6">
         <v>46447</v>
@@ -2419,7 +2419,7 @@
         <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G78" s="6">
         <v>46447</v>
@@ -2439,7 +2439,7 @@
         <v>210</v>
       </c>
       <c r="B80" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C80" t="s">
         <v>11</v>
@@ -2448,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G80" s="6">
         <v>39173</v>
@@ -2460,13 +2460,13 @@
         <v>433</v>
       </c>
       <c r="B81" t="s">
+        <v>155</v>
+      </c>
+      <c r="C81" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81" t="s">
         <v>156</v>
-      </c>
-      <c r="C81" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" t="s">
-        <v>157</v>
       </c>
       <c r="G81" s="6">
         <v>39539</v>
@@ -2479,7 +2479,7 @@
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2494,7 +2494,7 @@
         <v>208</v>
       </c>
       <c r="B84" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C84" t="s">
         <v>11</v>
@@ -2503,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="F84" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G84" s="6">
         <v>39539</v>
@@ -2573,7 +2573,7 @@
         <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G89" s="6">
         <v>46813</v>
@@ -2596,7 +2596,7 @@
         <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G90" s="6">
         <v>46813</v>
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="F104" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G104" s="6">
         <v>47178</v>
@@ -2806,16 +2806,16 @@
         <v>502</v>
       </c>
       <c r="B105" t="s">
+        <v>166</v>
+      </c>
+      <c r="C105" t="s">
         <v>167</v>
-      </c>
-      <c r="C105" t="s">
-        <v>168</v>
       </c>
       <c r="E105">
         <v>1</v>
       </c>
       <c r="F105" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G105" s="6">
         <v>39539</v>
@@ -2846,7 +2846,7 @@
         <v>7</v>
       </c>
       <c r="F108" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G108" s="6">
         <v>47178</v>
@@ -2900,13 +2900,13 @@
         <v>191</v>
       </c>
       <c r="B111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C111" t="s">
         <v>7</v>
       </c>
       <c r="F111" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G111" s="6">
         <v>39904</v>
@@ -2917,7 +2917,7 @@
         <v>137</v>
       </c>
       <c r="B112" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C112" t="s">
         <v>11</v>
@@ -2926,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="F112" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G112" s="6">
         <v>39904</v>
@@ -2996,10 +2996,13 @@
         <v>1</v>
       </c>
       <c r="F117" t="s">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="G117" s="6">
         <v>11383</v>
+      </c>
+      <c r="H117" s="6">
+        <v>39904</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -3007,16 +3010,19 @@
         <v>322</v>
       </c>
       <c r="B118" t="s">
+        <v>120</v>
+      </c>
+      <c r="C118" t="s">
+        <v>11</v>
+      </c>
+      <c r="F118" t="s">
         <v>121</v>
-      </c>
-      <c r="C118" t="s">
-        <v>11</v>
-      </c>
-      <c r="F118" t="s">
-        <v>122</v>
       </c>
       <c r="G118" s="6">
         <v>37347</v>
+      </c>
+      <c r="H118" s="6">
+        <v>39904</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
@@ -3024,7 +3030,7 @@
         <v>300</v>
       </c>
       <c r="B119" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C119" t="s">
         <v>11</v>
@@ -3038,7 +3044,7 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C120" t="s">
         <v>11</v>
@@ -3047,7 +3053,7 @@
         <v>1</v>
       </c>
       <c r="F120" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G120" s="6">
         <v>37712</v>
@@ -3061,13 +3067,13 @@
         <v>63</v>
       </c>
       <c r="B121" t="s">
+        <v>125</v>
+      </c>
+      <c r="C121" t="s">
+        <v>11</v>
+      </c>
+      <c r="F121" t="s">
         <v>126</v>
-      </c>
-      <c r="C121" t="s">
-        <v>11</v>
-      </c>
-      <c r="F121" t="s">
-        <v>127</v>
       </c>
       <c r="G121" s="6">
         <v>37712</v>
@@ -3081,13 +3087,13 @@
         <v>97</v>
       </c>
       <c r="B122" t="s">
+        <v>127</v>
+      </c>
+      <c r="C122" t="s">
+        <v>11</v>
+      </c>
+      <c r="F122" t="s">
         <v>128</v>
-      </c>
-      <c r="C122" t="s">
-        <v>11</v>
-      </c>
-      <c r="F122" t="s">
-        <v>129</v>
       </c>
       <c r="G122" s="6">
         <v>38078</v>
@@ -3245,7 +3251,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H116">
+  <conditionalFormatting sqref="H116:H118">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3294,17 +3300,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
careful thinking is required
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F95BA9-2FE6-B945-B054-CECFF26D1DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7342B2E-1D64-B240-B24F-59EE1AD3C21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12120" yWindow="760" windowWidth="22440" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="193">
   <si>
     <t>Note</t>
   </si>
@@ -613,6 +613,9 @@
   </si>
   <si>
     <t>Getting possible furtherest jump</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -680,7 +683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -692,6 +695,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1370,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1401,7 +1405,7 @@
       </c>
       <c r="G1" s="8">
         <f>COUNTA(G2:I179)</f>
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -3206,9 +3210,6 @@
       <c r="C123" t="s">
         <v>11</v>
       </c>
-      <c r="E123">
-        <v>1</v>
-      </c>
       <c r="F123" t="s">
         <v>124</v>
       </c>
@@ -3217,6 +3218,9 @@
       </c>
       <c r="H123" s="6">
         <v>38078</v>
+      </c>
+      <c r="I123" s="6">
+        <v>43191</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -3237,6 +3241,9 @@
       </c>
       <c r="H124" s="6">
         <v>38078</v>
+      </c>
+      <c r="I124" s="9" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -3368,7 +3375,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H123">
+  <conditionalFormatting sqref="H123:I123">
     <cfRule type="cellIs" dxfId="29" priority="30" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
i dont get it
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7342B2E-1D64-B240-B24F-59EE1AD3C21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CA014C-1327-EA4A-9F34-D90F9E21A3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12120" yWindow="760" windowWidth="22440" windowHeight="20540" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -1374,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="G1" s="8">
         <f>COUNTA(G2:I179)</f>
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2888,6 +2888,9 @@
       <c r="G102" s="6">
         <v>46813</v>
       </c>
+      <c r="H102" s="6">
+        <v>43191</v>
+      </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103">
@@ -2904,6 +2907,9 @@
       </c>
       <c r="G103" s="6">
         <v>47178</v>
+      </c>
+      <c r="H103" s="6">
+        <v>43191</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
@@ -3465,7 +3471,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H100:H101">
+  <conditionalFormatting sqref="H100:H103">
     <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
buble sort is slow
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/leetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E609CBF0-5285-AB4B-9620-E9CB76DA0A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A827BE5-BAF7-1144-8112-F02E6A24F7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20580" xr2:uid="{5D052A5D-2D4F-E348-A1FB-5A00C37AFAC8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="243">
   <si>
     <t>Note</t>
   </si>
@@ -764,6 +764,9 @@
   </si>
   <si>
     <t>기타</t>
+  </si>
+  <si>
+    <t>Sort List</t>
   </si>
 </sst>
 </file>
@@ -848,7 +851,27 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1111,11 +1134,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1131,11 +1154,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1449,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43C2F7-E3E5-DE49-B4C7-4EA3A8811DB9}">
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K103" sqref="K103"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1481,8 +1504,8 @@
         <v>0</v>
       </c>
       <c r="G1" s="1">
-        <f>COUNTA(G2:I192)</f>
-        <v>166</v>
+        <f>COUNTA(G2:I193)</f>
+        <v>168</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -3106,55 +3129,50 @@
       <c r="G105" s="6">
         <v>46813</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1" t="s">
+      <c r="H105" s="6">
+        <v>39234</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>148</v>
+      </c>
+      <c r="B106" t="s">
+        <v>242</v>
+      </c>
+      <c r="C106" t="s">
+        <v>12</v>
+      </c>
+      <c r="G106" s="6">
+        <v>39234</v>
+      </c>
+      <c r="H106" s="6"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-      <c r="F107" s="1"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="1"/>
-      <c r="I107" s="1"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <v>35</v>
-      </c>
-      <c r="B108" t="s">
-        <v>93</v>
-      </c>
-      <c r="C108" t="s">
-        <v>8</v>
-      </c>
-      <c r="F108" t="s">
-        <v>94</v>
-      </c>
-      <c r="G108" s="6">
-        <v>46813</v>
-      </c>
-      <c r="H108" s="6">
-        <v>39539</v>
-      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="B109" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C109" t="s">
-        <v>12</v>
-      </c>
-      <c r="D109">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F109" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G109" s="6">
         <v>46813</v>
@@ -3165,16 +3183,19 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="B110" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C110" t="s">
         <v>12</v>
       </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
       <c r="F110" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G110" s="6">
         <v>46813</v>
@@ -3185,39 +3206,39 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="B111" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C111" t="s">
         <v>12</v>
       </c>
       <c r="F111" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G111" s="6">
         <v>46813</v>
       </c>
       <c r="H111" s="6">
-        <v>43191</v>
+        <v>39539</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B112" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C112" t="s">
         <v>12</v>
       </c>
       <c r="F112" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G112" s="6">
-        <v>47178</v>
+        <v>46813</v>
       </c>
       <c r="H112" s="6">
         <v>43191</v>
@@ -3225,70 +3246,67 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113">
+        <v>34</v>
+      </c>
+      <c r="B113" t="s">
+        <v>101</v>
+      </c>
+      <c r="C113" t="s">
+        <v>12</v>
+      </c>
+      <c r="F113" t="s">
+        <v>102</v>
+      </c>
+      <c r="G113" s="6">
+        <v>47178</v>
+      </c>
+      <c r="H113" s="6">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114">
         <v>540</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>203</v>
       </c>
-      <c r="C113" t="s">
-        <v>12</v>
-      </c>
-      <c r="F113" t="s">
+      <c r="C114" t="s">
+        <v>12</v>
+      </c>
+      <c r="F114" t="s">
         <v>204</v>
       </c>
-      <c r="G113" s="6">
+      <c r="G114" s="6">
         <v>45383</v>
       </c>
-      <c r="H113" s="6"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1" t="s">
+      <c r="H114" s="6"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="5"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="1"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A116">
-        <v>215</v>
-      </c>
-      <c r="B116" t="s">
-        <v>104</v>
-      </c>
-      <c r="C116" t="s">
-        <v>12</v>
-      </c>
-      <c r="F116" t="s">
-        <v>105</v>
-      </c>
-      <c r="G116" s="6">
-        <v>47178</v>
-      </c>
-      <c r="H116" s="6">
-        <v>39539</v>
-      </c>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>373</v>
+        <v>215</v>
       </c>
       <c r="B117" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C117" t="s">
         <v>12</v>
       </c>
-      <c r="E117">
-        <v>1</v>
-      </c>
       <c r="F117" t="s">
-        <v>163</v>
+        <v>105</v>
       </c>
       <c r="G117" s="6">
         <v>47178</v>
@@ -3299,73 +3317,76 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>502</v>
+        <v>373</v>
       </c>
       <c r="B118" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="C118" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
       <c r="E118">
         <v>1</v>
       </c>
       <c r="F118" t="s">
+        <v>163</v>
+      </c>
+      <c r="G118" s="6">
+        <v>47178</v>
+      </c>
+      <c r="H118" s="6">
+        <v>39539</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>502</v>
+      </c>
+      <c r="B119" t="s">
+        <v>164</v>
+      </c>
+      <c r="C119" t="s">
+        <v>165</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="F119" t="s">
         <v>166</v>
       </c>
-      <c r="G118" s="6">
+      <c r="G119" s="6">
         <v>39539</v>
       </c>
-      <c r="H118" s="6"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1" t="s">
+      <c r="H119" s="6"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C120" s="1"/>
-      <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
-      <c r="F120" s="1"/>
-      <c r="G120" s="5"/>
-      <c r="H120" s="1"/>
-      <c r="I120" s="1"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A121">
-        <v>67</v>
-      </c>
-      <c r="B121" t="s">
-        <v>108</v>
-      </c>
-      <c r="C121" t="s">
-        <v>8</v>
-      </c>
-      <c r="F121" t="s">
-        <v>167</v>
-      </c>
-      <c r="G121" s="6">
-        <v>47178</v>
-      </c>
-      <c r="H121" s="6">
-        <v>39904</v>
-      </c>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>190</v>
+        <v>67</v>
       </c>
       <c r="B122" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C122" t="s">
         <v>8</v>
       </c>
       <c r="F122" t="s">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="G122" s="6">
-        <v>11018</v>
+        <v>47178</v>
       </c>
       <c r="H122" s="6">
         <v>39904</v>
@@ -3373,16 +3394,16 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>136</v>
+        <v>190</v>
       </c>
       <c r="B123" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C123" t="s">
         <v>8</v>
       </c>
       <c r="F123" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G123" s="6">
         <v>11018</v>
@@ -3393,83 +3414,83 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>191</v>
+        <v>136</v>
       </c>
       <c r="B124" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="C124" t="s">
         <v>8</v>
       </c>
       <c r="F124" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="G124" s="6">
+        <v>11018</v>
+      </c>
+      <c r="H124" s="6">
         <v>39904</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>137</v>
+        <v>191</v>
       </c>
       <c r="B125" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C125" t="s">
-        <v>12</v>
-      </c>
-      <c r="E125">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F125" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G125" s="6">
         <v>39904</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1" t="s">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>137</v>
+      </c>
+      <c r="B126" t="s">
+        <v>169</v>
+      </c>
+      <c r="C126" t="s">
+        <v>12</v>
+      </c>
+      <c r="E126">
+        <v>1</v>
+      </c>
+      <c r="F126" t="s">
+        <v>171</v>
+      </c>
+      <c r="G126" s="6">
+        <v>39904</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C127" s="1"/>
-      <c r="D127" s="1"/>
-      <c r="E127" s="1"/>
-      <c r="F127" s="1"/>
-      <c r="G127" s="5"/>
-      <c r="H127" s="1"/>
-      <c r="I127" s="1"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A128">
-        <v>70</v>
-      </c>
-      <c r="B128" t="s">
-        <v>114</v>
-      </c>
-      <c r="C128" t="s">
-        <v>8</v>
-      </c>
-      <c r="G128" s="6">
-        <v>11018</v>
-      </c>
-      <c r="H128" s="6">
-        <v>39904</v>
-      </c>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="5"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>198</v>
+        <v>70</v>
       </c>
       <c r="B129" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C129" t="s">
-        <v>12</v>
-      </c>
-      <c r="F129" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="G129" s="6">
         <v>11018</v>
@@ -3480,22 +3501,19 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>139</v>
+        <v>198</v>
       </c>
       <c r="B130" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C130" t="s">
         <v>12</v>
       </c>
-      <c r="E130">
-        <v>1</v>
-      </c>
       <c r="F130" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="G130" s="6">
-        <v>11383</v>
+        <v>11018</v>
       </c>
       <c r="H130" s="6">
         <v>39904</v>
@@ -3503,19 +3521,22 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>322</v>
+        <v>139</v>
       </c>
       <c r="B131" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C131" t="s">
         <v>12</v>
       </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
       <c r="F131" t="s">
-        <v>119</v>
+        <v>172</v>
       </c>
       <c r="G131" s="6">
-        <v>37347</v>
+        <v>11383</v>
       </c>
       <c r="H131" s="6">
         <v>39904</v>
@@ -3523,56 +3544,53 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>300</v>
+        <v>322</v>
       </c>
       <c r="B132" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C132" t="s">
         <v>12</v>
+      </c>
+      <c r="F132" t="s">
+        <v>119</v>
       </c>
       <c r="G132" s="6">
         <v>37347</v>
       </c>
       <c r="H132" s="6">
-        <v>43191</v>
+        <v>39904</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133">
+        <v>300</v>
+      </c>
+      <c r="B133" t="s">
         <v>120</v>
       </c>
-      <c r="B133" t="s">
-        <v>121</v>
-      </c>
       <c r="C133" t="s">
         <v>12</v>
       </c>
-      <c r="F133" t="s">
-        <v>122</v>
-      </c>
       <c r="G133" s="6">
-        <v>37712</v>
+        <v>37347</v>
       </c>
       <c r="H133" s="6">
-        <v>38078</v>
-      </c>
-      <c r="I133" s="8" t="s">
-        <v>190</v>
+        <v>43191</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="B134" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C134" t="s">
         <v>12</v>
       </c>
       <c r="F134" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G134" s="6">
         <v>37712</v>
@@ -3580,50 +3598,53 @@
       <c r="H134" s="6">
         <v>38078</v>
       </c>
+      <c r="I134" s="8" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="B135" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C135" t="s">
         <v>12</v>
       </c>
       <c r="F135" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G135" s="6">
+        <v>37712</v>
+      </c>
+      <c r="H135" s="6">
         <v>38078</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136">
-        <v>1143</v>
+        <v>97</v>
       </c>
       <c r="B136" t="s">
-        <v>193</v>
+        <v>125</v>
       </c>
       <c r="C136" t="s">
         <v>12</v>
       </c>
-      <c r="E136">
-        <v>1</v>
-      </c>
       <c r="F136" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
       <c r="G136" s="6">
-        <v>43556</v>
+        <v>38078</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137">
-        <v>72</v>
+        <v>1143</v>
       </c>
       <c r="B137" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C137" t="s">
         <v>12</v>
@@ -3632,85 +3653,91 @@
         <v>1</v>
       </c>
       <c r="F137" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G137" s="6">
         <v>43556</v>
       </c>
-      <c r="H137" s="6">
-        <v>44652</v>
-      </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>221</v>
+        <v>72</v>
       </c>
       <c r="B138" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C138" t="s">
         <v>12</v>
       </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
       <c r="F138" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G138" s="6">
-        <v>43922</v>
+        <v>43556</v>
+      </c>
+      <c r="H138" s="6">
+        <v>44652</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139">
+        <v>221</v>
+      </c>
+      <c r="B139" t="s">
+        <v>197</v>
+      </c>
+      <c r="C139" t="s">
+        <v>12</v>
+      </c>
+      <c r="F139" t="s">
+        <v>198</v>
+      </c>
+      <c r="G139" s="6">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A140">
         <v>64</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" t="s">
         <v>218</v>
       </c>
-      <c r="C139" t="s">
-        <v>12</v>
-      </c>
-      <c r="F139" t="s">
+      <c r="C140" t="s">
+        <v>12</v>
+      </c>
+      <c r="F140" t="s">
         <v>219</v>
       </c>
-      <c r="G139" s="6">
+      <c r="G140" s="6">
         <v>44317</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A141" s="1"/>
-      <c r="B141" s="1" t="s">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C141" s="1"/>
-      <c r="D141" s="1"/>
-      <c r="E141" s="1"/>
-      <c r="F141" s="1"/>
-      <c r="G141" s="5"/>
-      <c r="H141" s="1"/>
-      <c r="I141" s="1"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B142" t="s">
-        <v>175</v>
-      </c>
-      <c r="C142" t="s">
-        <v>12</v>
-      </c>
-      <c r="F142" t="s">
-        <v>176</v>
-      </c>
-      <c r="G142" s="6">
-        <v>41365</v>
-      </c>
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="5"/>
+      <c r="H142" s="1"/>
+      <c r="I142" s="1"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C143" t="s">
         <v>12</v>
       </c>
       <c r="F143" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G143" s="6">
         <v>41365</v>
@@ -3718,13 +3745,13 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C144" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F144" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G144" s="6">
         <v>41365</v>
@@ -3732,13 +3759,13 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C145" t="s">
         <v>8</v>
       </c>
       <c r="F145" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G145" s="6">
         <v>41365</v>
@@ -3746,7 +3773,13 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
-        <v>184</v>
+        <v>182</v>
+      </c>
+      <c r="C146" t="s">
+        <v>8</v>
+      </c>
+      <c r="F146" t="s">
+        <v>183</v>
       </c>
       <c r="G146" s="6">
         <v>41365</v>
@@ -3754,163 +3787,181 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G147" s="6">
         <v>41365</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A149" s="1"/>
-      <c r="B149" s="1" t="s">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B148" t="s">
+        <v>185</v>
+      </c>
+      <c r="G148" s="6">
+        <v>41365</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C149" s="1"/>
-      <c r="D149" s="1"/>
-      <c r="E149" s="1"/>
-      <c r="F149" s="1"/>
-      <c r="G149" s="5"/>
-      <c r="H149" s="1"/>
-      <c r="I149" s="1"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="5"/>
+      <c r="H150" s="1"/>
+      <c r="I150" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="28" priority="55" operator="equal">
-      <formula>"Easy"</formula>
+    <cfRule type="cellIs" dxfId="30" priority="55" operator="equal">
+      <formula>"Hard"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="56" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="53" operator="equal">
-      <formula>"Hard"</formula>
+    <cfRule type="cellIs" dxfId="28" priority="57" operator="equal">
+      <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F45 D1:E74 F49:F74 D71:F1048576">
-    <cfRule type="cellIs" dxfId="25" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="54" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G48 G50:G1048576">
-    <cfRule type="cellIs" dxfId="24" priority="56" stopIfTrue="1" operator="greaterThan">
+  <conditionalFormatting sqref="G2:G48 G50:G105 G107:G1048576">
+    <cfRule type="cellIs" dxfId="26" priority="58" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="23" priority="51" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="53" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H34">
-    <cfRule type="cellIs" dxfId="22" priority="16" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="18" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="cellIs" dxfId="21" priority="21" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="23" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44:H46">
-    <cfRule type="cellIs" dxfId="20" priority="13" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="15" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51:H54">
-    <cfRule type="cellIs" dxfId="19" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="14" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64:H69">
-    <cfRule type="cellIs" dxfId="17" priority="9" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="11" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77:H81">
-    <cfRule type="cellIs" dxfId="16" priority="7" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="9" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84:H87">
-    <cfRule type="cellIs" dxfId="15" priority="5" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="7" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89:H94">
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H100:H102">
-    <cfRule type="cellIs" dxfId="13" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H108:H113">
-    <cfRule type="cellIs" dxfId="12" priority="18" stopIfTrue="1" operator="greaterThan">
+  <conditionalFormatting sqref="H109:H114">
+    <cfRule type="cellIs" dxfId="14" priority="20" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H116:H118">
-    <cfRule type="cellIs" dxfId="11" priority="31" stopIfTrue="1" operator="greaterThan">
+  <conditionalFormatting sqref="H117:H119">
+    <cfRule type="cellIs" dxfId="13" priority="33" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H121:H123">
-    <cfRule type="cellIs" dxfId="10" priority="28" stopIfTrue="1" operator="greaterThan">
+  <conditionalFormatting sqref="H122:H124">
+    <cfRule type="cellIs" dxfId="12" priority="30" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H128:H134">
+  <conditionalFormatting sqref="H129:H135">
+    <cfRule type="cellIs" dxfId="11" priority="27" stopIfTrue="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H138">
+    <cfRule type="cellIs" dxfId="10" priority="21" stopIfTrue="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:I15">
     <cfRule type="cellIs" dxfId="9" priority="25" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H137">
-    <cfRule type="cellIs" dxfId="8" priority="19" stopIfTrue="1" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:I15">
-    <cfRule type="cellIs" dxfId="7" priority="23" stopIfTrue="1" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H99:I99">
-    <cfRule type="cellIs" dxfId="6" priority="35" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="37" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
-    <cfRule type="cellIs" dxfId="5" priority="14" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="16" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54">
-    <cfRule type="cellIs" dxfId="4" priority="11" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="13" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I78">
-    <cfRule type="cellIs" dxfId="3" priority="8" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="10" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I84">
-    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="8" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I89">
-    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I101:I102">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H105:H106">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G106">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>